<commit_message>
half-maximal cell growth: from mmHg to mMol/L O2
</commit_message>
<xml_diff>
--- a/data/S-phase_duration_Params.xlsx
+++ b/data/S-phase_duration_Params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/4470246/Projects/PMO/HighPloidy_DoubleEdgedSword/code/MathModel/GrowOrGo_PloidyEnergyRobustness/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D8280-9500-1C40-9B30-E1ECDAFBED57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B578E528-3427-084F-A394-657B7AF9C4F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="32360" windowHeight="18860" xr2:uid="{DA59BEBD-339E-6640-84EB-F8DDFB9BD691}"/>
+    <workbookView xWindow="10760" yWindow="7700" windowWidth="32360" windowHeight="18820" xr2:uid="{DA59BEBD-339E-6640-84EB-F8DDFB9BD691}"/>
   </bookViews>
   <sheets>
     <sheet name="Params" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>T1</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>24068884</t>
+  </si>
+  <si>
+    <t>coefficient of O2 solubility in water</t>
+  </si>
+  <si>
+    <t>mMol*L^-1 *mmHg^-1</t>
+  </si>
+  <si>
+    <t>mMol*L^-1</t>
+  </si>
+  <si>
+    <t>Henry's law</t>
+  </si>
+  <si>
+    <t>12771568</t>
   </si>
 </sst>
 </file>
@@ -567,15 +582,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84648E7-4A5B-F642-80F8-159A6E3CA6CA}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="10" style="6" customWidth="1"/>
@@ -767,11 +782,11 @@
         <v>39</v>
       </c>
       <c r="B13">
-        <f>0.009241*B15</f>
-        <v>7.023159999999999</v>
+        <f>0.009241*B15*B16</f>
+        <v>9.7621923999999978E-3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>43</v>
@@ -813,6 +828,24 @@
       </c>
       <c r="E15" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <f>1.39*10^-3</f>
+        <v>1.39E-3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>